<commit_message>
V1.0 Build and Bug fixes following fault finding
</commit_message>
<xml_diff>
--- a/keyboardLayoutEditor/switchLayout2.xlsx
+++ b/keyboardLayoutEditor/switchLayout2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\a2000Serotina\a2000Serotina\keyboardLayoutEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A671604A-D6EE-4E91-B42C-2CA88CD4EB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160EA602-01F1-4DF6-AA74-045E6F6189E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="1485" windowWidth="31455" windowHeight="17445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,11 +2309,8 @@
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2335,11 +2332,8 @@
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>225</v>
-      </c>
-      <c r="L43" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2359,7 +2353,9 @@
       <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C45" s="1" t="s">
         <v>82</v>
       </c>
@@ -2384,6 +2380,9 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>226</v>
+      </c>
       <c r="C46" t="s">
         <v>227</v>
       </c>

</xml_diff>